<commit_message>
Nettoyage structure + affichage prix laiton OK
</commit_message>
<xml_diff>
--- a/prix/laiton.xlsx
+++ b/prix/laiton.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\raccords-plomberie\prix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7285FE27-258F-4AFB-83D0-2FACD4D97977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C52AD-869F-468E-9BF6-D1393D928E1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2BA8A27F-C677-4342-8A29-D0C4A22FC515}"/>
   </bookViews>
@@ -1052,7 +1052,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1075,6 +1075,12 @@
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1413,14 +1419,14 @@
   <dimension ref="A1:N127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C127"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" style="10" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.77734375" style="1" customWidth="1"/>
@@ -1439,7 +1445,7 @@
       <c r="B1" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="9" t="s">
         <v>251</v>
       </c>
       <c r="D1" s="5" t="s">

</xml_diff>